<commit_message>
Completed first four lessons of python course and updated SQL project.
</commit_message>
<xml_diff>
--- a/SQL-Python-Git/SQL/SQL Project/1 - Plot/top-5-month-to-month.xlsx
+++ b/SQL-Python-Git/SQL/SQL Project/1 - Plot/top-5-month-to-month.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d9df4817efbddffa/Documents/Ryan/Career Change/03. Data Science - Udacity/01. Python and SQL/SQL-Python-Git/SQL/SQL Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ihscourse\Desktop\Data Science - Udacity\SQL-Python-Git\SQL\SQL Project\1 - Plot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{61CBFCDD-4D36-4FF5-8DE8-330B55DD9239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BA439D-EA29-48BC-909B-65D3553B044B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="735" yWindow="735" windowWidth="13665" windowHeight="12225"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="top-5-month-to-month" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>rental_date</t>
   </si>
@@ -39,11 +39,14 @@
   <si>
     <t>mexico</t>
   </si>
+  <si>
+    <t>=</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -599,8 +602,9 @@
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -617,11 +621,34 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst>
               <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
@@ -631,9 +658,7 @@
               </a:outerShdw>
             </a:effectLst>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'top-5-month-to-month'!$A$2:$A$5</c:f>
@@ -676,7 +701,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-724A-489D-9220-1D165DEBAD01}"/>
@@ -698,11 +722,34 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst>
               <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
@@ -712,9 +759,7 @@
               </a:outerShdw>
             </a:effectLst>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'top-5-month-to-month'!$A$2:$A$5</c:f>
@@ -757,7 +802,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-724A-489D-9220-1D165DEBAD01}"/>
@@ -779,11 +823,34 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst>
               <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
@@ -793,9 +860,7 @@
               </a:outerShdw>
             </a:effectLst>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'top-5-month-to-month'!$A$2:$A$5</c:f>
@@ -838,7 +903,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-724A-489D-9220-1D165DEBAD01}"/>
@@ -860,11 +924,34 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst>
               <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
@@ -874,9 +961,7 @@
               </a:outerShdw>
             </a:effectLst>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'top-5-month-to-month'!$A$2:$A$5</c:f>
@@ -919,7 +1004,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-724A-489D-9220-1D165DEBAD01}"/>
@@ -941,11 +1025,34 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst>
               <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
@@ -955,9 +1062,7 @@
               </a:outerShdw>
             </a:effectLst>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'top-5-month-to-month'!$A$2:$A$5</c:f>
@@ -1000,7 +1105,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-724A-489D-9220-1D165DEBAD01}"/>
@@ -1015,10 +1119,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
+        <c:gapWidth val="150"/>
         <c:axId val="514628344"/>
         <c:axId val="514626744"/>
-      </c:lineChart>
+      </c:barChart>
       <c:catAx>
         <c:axId val="514628344"/>
         <c:scaling>
@@ -1026,6 +1130,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Month</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1091,6 +1250,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Rentals</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1124,7 +1338,7 @@
         </c:txPr>
         <c:crossAx val="514628344"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2088,16 +2302,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AA38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="56" workbookViewId="0">
-      <selection activeCell="W38" sqref="W38"/>
+      <selection activeCell="AC32" sqref="AC32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2117,7 +2331,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44686</v>
       </c>
@@ -2137,7 +2351,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44718</v>
       </c>
@@ -2157,7 +2371,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44749</v>
       </c>
@@ -2177,7 +2391,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44781</v>
       </c>
@@ -2195,6 +2409,11 @@
       </c>
       <c r="F5">
         <v>311</v>
+      </c>
+    </row>
+    <row r="38" spans="27:27" x14ac:dyDescent="0.3">
+      <c r="AA38" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>